<commit_message>
Updating lab 3 calculations and data
</commit_message>
<xml_diff>
--- a/335Lab/Lab 3/rawData/Unit2 Edited.xlsx
+++ b/335Lab/Lab 3/rawData/Unit2 Edited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Class Work\Current\ME335\335Lab\Lab 3\rawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46E5276-34AA-43E2-A37F-D9EB68F70AA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18006AE-0A7D-4D24-857E-AFE46FCFEC79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1019,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J198"/>
+  <dimension ref="A1:J199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,6 +1284,14 @@
       <c r="E15">
         <v>47.85</v>
       </c>
+      <c r="F15">
+        <f>_xlfn.STDEV.S(D10:D14)</f>
+        <v>0.61808575456808545</v>
+      </c>
+      <c r="G15">
+        <f>_xlfn.STDEV.S(E10:E14)</f>
+        <v>9.5812316536027828E-2</v>
+      </c>
       <c r="I15" t="s">
         <v>33</v>
       </c>
@@ -1404,6 +1412,14 @@
       <c r="E20">
         <v>47.85</v>
       </c>
+      <c r="F20">
+        <f>_xlfn.STDEV.S(D15:D19)</f>
+        <v>0.95223421488623394</v>
+      </c>
+      <c r="G20">
+        <f>_xlfn.STDEV.S(E15:E19)</f>
+        <v>7.5033325929214939E-2</v>
+      </c>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1498,6 +1514,14 @@
       <c r="E25">
         <v>47.8</v>
       </c>
+      <c r="F25">
+        <f>_xlfn.STDEV.S(D20:D24)</f>
+        <v>0.58579006478430684</v>
+      </c>
+      <c r="G25">
+        <f>_xlfn.STDEV.S(E20:E24)</f>
+        <v>4.3243496620878424E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -1591,6 +1615,14 @@
       <c r="E30">
         <v>47.84</v>
       </c>
+      <c r="F30">
+        <f>_xlfn.STDEV.S(D25:D29)</f>
+        <v>0.90483700189591587</v>
+      </c>
+      <c r="G30">
+        <f>_xlfn.STDEV.S(E25:E29)</f>
+        <v>5.2630789467762389E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -1684,6 +1716,14 @@
       <c r="E35">
         <v>47.93</v>
       </c>
+      <c r="F35">
+        <f>_xlfn.STDEV.S(D30:D34)</f>
+        <v>6.8159848884808998</v>
+      </c>
+      <c r="G35">
+        <f>_xlfn.STDEV.S(E30:E34)</f>
+        <v>8.7349871207690624E-2</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -1777,6 +1817,14 @@
       <c r="E40">
         <v>47.84</v>
       </c>
+      <c r="F40">
+        <f>_xlfn.STDEV.S(D35:D39)</f>
+        <v>1.9994824330311083</v>
+      </c>
+      <c r="G40">
+        <f>_xlfn.STDEV.S(E35:E39)</f>
+        <v>0.14300349646075278</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -1870,6 +1918,14 @@
       <c r="E45">
         <v>47.63</v>
       </c>
+      <c r="F45">
+        <f>_xlfn.STDEV.S(D40:D44)</f>
+        <v>0.50707987536481469</v>
+      </c>
+      <c r="G45">
+        <f>_xlfn.STDEV.S(E40:E44)</f>
+        <v>4.4944410108488694E-2</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -1963,6 +2019,14 @@
       <c r="E50">
         <v>47.92</v>
       </c>
+      <c r="F50">
+        <f>_xlfn.STDEV.S(D45:D49)</f>
+        <v>1.0803101406540592</v>
+      </c>
+      <c r="G50">
+        <f>_xlfn.STDEV.S(E45:E49)</f>
+        <v>8.8204308284797778E-2</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
@@ -2040,6 +2104,16 @@
         <v>47.817999999999998</v>
       </c>
     </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <f>_xlfn.STDEV.S(D50:D54)</f>
+        <v>0.95276964687169663</v>
+      </c>
+      <c r="G55">
+        <f>_xlfn.STDEV.S(E50:E54)</f>
+        <v>0.10616025621672183</v>
+      </c>
+    </row>
     <row r="56" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B56" s="4" t="s">
         <v>21</v>
@@ -2206,6 +2280,14 @@
       <c r="E63">
         <v>39.799999999999997</v>
       </c>
+      <c r="F63">
+        <f>_xlfn.STDEV.S(D58:D62)</f>
+        <v>0.6026192827980198</v>
+      </c>
+      <c r="G63">
+        <f>_xlfn.STDEV.S(E58:E62)</f>
+        <v>0.11238327277669095</v>
+      </c>
       <c r="I63" t="s">
         <v>33</v>
       </c>
@@ -2326,6 +2408,14 @@
       <c r="E68">
         <v>39.799999999999997</v>
       </c>
+      <c r="F68">
+        <f>_xlfn.STDEV.S(D63:D67)</f>
+        <v>0.66389005113799093</v>
+      </c>
+      <c r="G68">
+        <f>_xlfn.STDEV.S(E63:E67)</f>
+        <v>5.4037024344424693E-2</v>
+      </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
@@ -2419,6 +2509,14 @@
       <c r="E73">
         <v>39.65</v>
       </c>
+      <c r="F73">
+        <f>_xlfn.STDEV.S(D68:D72)</f>
+        <v>0.80729176881719866</v>
+      </c>
+      <c r="G73">
+        <f>_xlfn.STDEV.S(E68:E72)</f>
+        <v>6.0249481325569558E-2</v>
+      </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
@@ -2512,6 +2610,14 @@
       <c r="E78">
         <v>39.75</v>
       </c>
+      <c r="F78">
+        <f>_xlfn.STDEV.S(D73:D77)</f>
+        <v>0.66281973416608353</v>
+      </c>
+      <c r="G78">
+        <f>_xlfn.STDEV.S(E73:E77)</f>
+        <v>5.9749476985158451E-2</v>
+      </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
@@ -2605,6 +2711,14 @@
       <c r="E83">
         <v>39.75</v>
       </c>
+      <c r="F83">
+        <f>_xlfn.STDEV.S(D78:D82)</f>
+        <v>5.3743492629340732</v>
+      </c>
+      <c r="G83">
+        <f>_xlfn.STDEV.S(E78:E82)</f>
+        <v>4.3243496620878674E-2</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
@@ -2698,6 +2812,14 @@
       <c r="E88">
         <v>39.96</v>
       </c>
+      <c r="F88">
+        <f>_xlfn.STDEV.S(D83:D87)</f>
+        <v>4.2501729376579469</v>
+      </c>
+      <c r="G88">
+        <f>_xlfn.STDEV.S(E83:E87)</f>
+        <v>4.2071367935925842E-2</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
@@ -2791,6 +2913,14 @@
       <c r="E93">
         <v>39.86</v>
       </c>
+      <c r="F93">
+        <f>_xlfn.STDEV.S(D88:D92)</f>
+        <v>1.2570322191574885</v>
+      </c>
+      <c r="G93">
+        <f>_xlfn.STDEV.S(E88:E92)</f>
+        <v>0.14310835055998794</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
@@ -2884,6 +3014,14 @@
       <c r="E98">
         <v>39.67</v>
       </c>
+      <c r="F98">
+        <f>_xlfn.STDEV.S(D93:D97)</f>
+        <v>0.82090194298710573</v>
+      </c>
+      <c r="G98">
+        <f>_xlfn.STDEV.S(E93:E97)</f>
+        <v>0.12557866060760406</v>
+      </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99">
@@ -2961,6 +3099,16 @@
         <v>39.655999999999999</v>
       </c>
     </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F103">
+        <f>_xlfn.STDEV.S(D98:D102)</f>
+        <v>0.81452440110778523</v>
+      </c>
+      <c r="G103">
+        <f>_xlfn.STDEV.S(E98:E102)</f>
+        <v>7.8612976028133275E-2</v>
+      </c>
+    </row>
     <row r="104" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B104" s="4" t="s">
         <v>22</v>
@@ -3128,6 +3276,14 @@
       <c r="E111">
         <v>31.84</v>
       </c>
+      <c r="F111">
+        <f>_xlfn.STDEV.S(D106:D110)</f>
+        <v>0.58044810276199865</v>
+      </c>
+      <c r="G111">
+        <f>_xlfn.STDEV.S(E106:E110)</f>
+        <v>7.4833147735479139E-2</v>
+      </c>
       <c r="I111" t="s">
         <v>33</v>
       </c>
@@ -3248,6 +3404,14 @@
       <c r="E116">
         <v>31.83</v>
       </c>
+      <c r="F116">
+        <f>_xlfn.STDEV.S(D111:D115)</f>
+        <v>0.44054511687226977</v>
+      </c>
+      <c r="G116">
+        <f>_xlfn.STDEV.S(E111:E115)</f>
+        <v>5.3572380943914651E-2</v>
+      </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117">
@@ -3341,6 +3505,14 @@
       <c r="E121">
         <v>31.75</v>
       </c>
+      <c r="F121">
+        <f>_xlfn.STDEV.S(D116:D120)</f>
+        <v>0.79772802382767094</v>
+      </c>
+      <c r="G121">
+        <f>_xlfn.STDEV.S(E116:E120)</f>
+        <v>6.5192024052026593E-2</v>
+      </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122">
@@ -3434,6 +3606,14 @@
       <c r="E126">
         <v>31.73</v>
       </c>
+      <c r="F126">
+        <f>_xlfn.STDEV.S(D121:D125)</f>
+        <v>0.43043001754059673</v>
+      </c>
+      <c r="G126">
+        <f>_xlfn.STDEV.S(E121:E125)</f>
+        <v>6.8920243760451055E-2</v>
+      </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127">
@@ -3527,6 +3707,14 @@
       <c r="E131">
         <v>31.87</v>
       </c>
+      <c r="F131">
+        <f>_xlfn.STDEV.S(D126:D130)</f>
+        <v>0.63885053024944638</v>
+      </c>
+      <c r="G131">
+        <f>_xlfn.STDEV.S(E126:E130)</f>
+        <v>3.8470768123341874E-2</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
@@ -3620,6 +3808,14 @@
       <c r="E136">
         <v>31.82</v>
       </c>
+      <c r="F136">
+        <f>_xlfn.STDEV.S(D131:D135)</f>
+        <v>0.9072210315022472</v>
+      </c>
+      <c r="G136">
+        <f>_xlfn.STDEV.S(E131:E135)</f>
+        <v>6.403124237432864E-2</v>
+      </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
@@ -3713,6 +3909,14 @@
       <c r="E141">
         <v>31.8</v>
       </c>
+      <c r="F141">
+        <f>_xlfn.STDEV.S(D136:D140)</f>
+        <v>0.42764471234893342</v>
+      </c>
+      <c r="G141">
+        <f>_xlfn.STDEV.S(E136:E140)</f>
+        <v>3.3615472627943302E-2</v>
+      </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
@@ -3806,6 +4010,14 @@
       <c r="E146">
         <v>31.85</v>
       </c>
+      <c r="F146">
+        <f>_xlfn.STDEV.S(D141:D145)</f>
+        <v>0.72818266939003684</v>
+      </c>
+      <c r="G146">
+        <f>_xlfn.STDEV.S(E141:E145)</f>
+        <v>5.8137767414995094E-2</v>
+      </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147">
@@ -3883,6 +4095,16 @@
         <v>31.731999999999999</v>
       </c>
     </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F151">
+        <f>_xlfn.STDEV.S(D146:D150)</f>
+        <v>0.38310572953168009</v>
+      </c>
+      <c r="G151">
+        <f>_xlfn.STDEV.S(E146:E150)</f>
+        <v>8.983317872590374E-2</v>
+      </c>
+    </row>
     <row r="152" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B152" s="4" t="s">
         <v>23</v>
@@ -4049,6 +4271,14 @@
       <c r="E159">
         <v>23.74</v>
       </c>
+      <c r="F159">
+        <f>_xlfn.STDEV.S(D154:D158)</f>
+        <v>0.69934254839813692</v>
+      </c>
+      <c r="G159">
+        <f>_xlfn.STDEV.S(E154:E158)</f>
+        <v>3.5777087639997658E-2</v>
+      </c>
       <c r="I159" t="s">
         <v>33</v>
       </c>
@@ -4169,6 +4399,14 @@
       <c r="E164">
         <v>23.71</v>
       </c>
+      <c r="F164">
+        <f>_xlfn.STDEV.S(D159:D163)</f>
+        <v>0.29507626132916831</v>
+      </c>
+      <c r="G164">
+        <f>_xlfn.STDEV.S(E159:E163)</f>
+        <v>7.0213958726167924E-2</v>
+      </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165">
@@ -4262,6 +4500,14 @@
       <c r="E169">
         <v>23.82</v>
       </c>
+      <c r="F169">
+        <f>_xlfn.STDEV.S(D164:D168)</f>
+        <v>0.22711230702011945</v>
+      </c>
+      <c r="G169">
+        <f>_xlfn.STDEV.S(E164:E168)</f>
+        <v>7.4632432628181214E-2</v>
+      </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170">
@@ -4355,6 +4601,14 @@
       <c r="E174">
         <v>23.79</v>
       </c>
+      <c r="F174">
+        <f>_xlfn.STDEV.S(D169:D173)</f>
+        <v>0.13630847369110907</v>
+      </c>
+      <c r="G174">
+        <f>_xlfn.STDEV.S(E169:E173)</f>
+        <v>4.6151923036857709E-2</v>
+      </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175">
@@ -4448,6 +4702,14 @@
       <c r="E179">
         <v>23.79</v>
       </c>
+      <c r="F179">
+        <f>_xlfn.STDEV.S(D174:D178)</f>
+        <v>0.43637140144606268</v>
+      </c>
+      <c r="G179">
+        <f>_xlfn.STDEV.S(E174:E178)</f>
+        <v>4.9699094559157574E-2</v>
+      </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
@@ -4541,6 +4803,14 @@
       <c r="E184">
         <v>23.74</v>
       </c>
+      <c r="F184">
+        <f>_xlfn.STDEV.S(D179:D183)</f>
+        <v>0.20305171754998907</v>
+      </c>
+      <c r="G184">
+        <f>_xlfn.STDEV.S(E179:E183)</f>
+        <v>6.5954529791363861E-2</v>
+      </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
@@ -4634,6 +4904,14 @@
       <c r="E189">
         <v>23.72</v>
       </c>
+      <c r="F189">
+        <f>_xlfn.STDEV.S(D184:D188)</f>
+        <v>0.3246074552440219</v>
+      </c>
+      <c r="G189">
+        <f>_xlfn.STDEV.S(E184:E188)</f>
+        <v>6.0580524923443131E-2</v>
+      </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
@@ -4727,6 +5005,14 @@
       <c r="E194">
         <v>23.63</v>
       </c>
+      <c r="F194">
+        <f>_xlfn.STDEV.S(D189:D193)</f>
+        <v>0.14567086187703876</v>
+      </c>
+      <c r="G194">
+        <f>_xlfn.STDEV.S(E189:E193)</f>
+        <v>4.472135954999603E-2</v>
+      </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
@@ -4802,6 +5088,16 @@
       <c r="G198">
         <f>AVERAGE(E194:E198)</f>
         <v>23.755999999999997</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F199">
+        <f>_xlfn.STDEV.S(D194:D198)</f>
+        <v>0.26884940022250448</v>
+      </c>
+      <c r="G199">
+        <f>_xlfn.STDEV.S(E194:E198)</f>
+        <v>7.7653074633268968E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4811,6 +5107,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C35235A0CBEA4E4BA44A492B72CB0F55" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70e5c958f602f45486ea9c9e3e1161eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6112e395-b193-4778-b513-460523810ab5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df585931453734ed62ad13ba882f2bc2" ns2:_="">
     <xsd:import namespace="6112e395-b193-4778-b513-460523810ab5"/>
@@ -4942,22 +5253,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97C955C-B26D-4F4C-B6C8-7D7043F58F97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A098506D-CC41-46F9-9D15-58AF44E9E5A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9609D135-251D-4F2A-AC96-B47EE691F24C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4973,21 +5286,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A098506D-CC41-46F9-9D15-58AF44E9E5A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97C955C-B26D-4F4C-B6C8-7D7043F58F97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>